<commit_message>
All accounts tests pass for inventory and livestock inventory
</commit_message>
<xml_diff>
--- a/libs/accounts/src/test/example_xlsx/Account-TEST-Bank.xlsx
+++ b/libs/accounts/src/test/example_xlsx/Account-TEST-Bank.xlsx
@@ -8,11 +8,11 @@
     <sheet state="visible" name="bank.creditcards" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_935CBEFF_E013_4D2F_AB51_8219ADF08BDF_.wvu.FilterData">bank.checking!$A$1:$M$240</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_8296872D_E3F9_4C98_96ED_3FF984AEA99B_.wvu.FilterData">bank.checking!$A$1:$M$240</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{935CBEFF-E013-4D2F-AB51-8219ADF08BDF}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8296872D-E3F9-4C98-96ED-3FF984AEA99B}" name="Filter 1"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -431,7 +431,7 @@
     <t>Cow Processor</t>
   </si>
   <si>
-    <t>head: 53; weight: 76850; outid: 2022-01-23_PROCESSOR1; latecash: true</t>
+    <t>head: 54; weight: 78300; outid: 2022-01-23_PROCESSOR1; latecash: true</t>
   </si>
   <si>
     <t>1242</t>
@@ -9770,7 +9770,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{935CBEFF-E013-4D2F-AB51-8219ADF08BDF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8296872D-E3F9-4C98-96ED-3FF984AEA99B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$M$240"/>
     </customSheetView>
   </customSheetViews>
@@ -9872,7 +9872,7 @@
       <c r="E2" s="85"/>
       <c r="F2" s="86">
         <f t="array" ref="F2">1000000-INDEX(J:J,MAX((J:J&lt;&gt;"")*(ROW(J:J))))</f>
-        <v>808443.71</v>
+        <v>810183.71</v>
       </c>
       <c r="G2" s="78"/>
       <c r="H2" s="10"/>
@@ -10634,12 +10634,12 @@
       </c>
       <c r="G23" s="78"/>
       <c r="H23" s="109">
-        <v>92220.0</v>
+        <v>93960.0</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="92">
         <f t="shared" si="1"/>
-        <v>217006.29</v>
+        <v>215266.29</v>
       </c>
       <c r="K23" s="77" t="s">
         <v>136</v>
@@ -10669,7 +10669,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="92">
         <f t="shared" si="1"/>
-        <v>204296.29</v>
+        <v>202556.29</v>
       </c>
       <c r="K24" s="77" t="s">
         <v>139</v>
@@ -10699,7 +10699,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="110">
         <f t="shared" si="1"/>
-        <v>191556.29</v>
+        <v>189816.29</v>
       </c>
       <c r="K25" s="77" t="s">
         <v>142</v>

</xml_diff>